<commit_message>
[232P] quiz2 checkout till lab3 and practice
</commit_message>
<xml_diff>
--- a/232P/lab3/lab3.xlsx
+++ b/232P/lab3/lab3.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ms@uci\232P\lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A4A184-62F9-42A9-8E45-5C9197ECD7BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F74F24-143E-48B6-9E47-A902CF50C51E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="-18915" windowWidth="28230" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="templates" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>R1</t>
   </si>
@@ -225,6 +226,12 @@
   </si>
   <si>
     <t>ipv6 route fd01:2345:6789:3::/64 f1/0 fd01:2345:6789:2::1</t>
+  </si>
+  <si>
+    <t>interface ROUTER_INTERFACE</t>
+  </si>
+  <si>
+    <t>ip address ROUTER_IP ROUTER_MASK</t>
   </si>
 </sst>
 </file>
@@ -278,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -286,6 +293,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:B46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,10 +771,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>46</v>
@@ -774,10 +782,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -841,9 +849,6 @@
       <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -852,9 +857,6 @@
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -863,9 +865,6 @@
       <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -874,27 +873,11 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -903,19 +886,6 @@
       <c r="B30" t="s">
         <v>50</v>
       </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1003,6 +973,178 @@
       </c>
       <c r="B46" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F87AAD-E4F3-4376-827F-36E18BEAD536}">
+  <dimension ref="A2:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE((SUBSTITUTE(A2,"ROUTER_INTERFACE","FastEther1/0")),"ROUTER_MASK","255.255255.0"), "ROUTER_IP", "10.0.1.1")</f>
+        <v>configure terminal</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B9" si="0">SUBSTITUTE(SUBSTITUTE((SUBSTITUTE(A3,"ROUTER_INTERFACE","FastEther1/0")),"ROUTER_MASK","255.255255.0"), "ROUTER_IP", "10.0.1.1")</f>
+        <v>no ip routing</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>ip routing</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>interface FastEther1/0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>ip address 10.0.1.1 255.255255.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>no shutdown</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>end</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>show ip interface brief</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f t="shared" ref="B3:B15" si="1">SUBSTITUTE((SUBSTITUTE(A11:A18,"ROUTER_INTERFACE","Serial2/0")),"ROUTER_MASK",255.255255)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>